<commit_message>
built the sythetic data but still needs more tweaking to be more real
</commit_message>
<xml_diff>
--- a/python/data_processing/output/consultancy_data.xlsx
+++ b/python/data_processing/output/consultancy_data.xlsx
@@ -1530,7 +1530,7 @@
         <v>31</v>
       </c>
       <c r="AC8" t="n">
-        <v>12.70735869059762</v>
+        <v>12.7</v>
       </c>
       <c r="AD8" t="n">
         <v>49</v>
@@ -2332,7 +2332,7 @@
         <v>32</v>
       </c>
       <c r="AC14" t="n">
-        <v>26.16500348718269</v>
+        <v>26.2</v>
       </c>
       <c r="AD14" t="n">
         <v>50</v>
@@ -3134,7 +3134,7 @@
         <v>37</v>
       </c>
       <c r="AC20" t="n">
-        <v>22.42547006934152</v>
+        <v>22.4</v>
       </c>
       <c r="AD20" t="n">
         <v>54</v>
@@ -3400,7 +3400,7 @@
         <v>34</v>
       </c>
       <c r="AC22" t="n">
-        <v>20.98394913738452</v>
+        <v>21</v>
       </c>
       <c r="AD22" t="n">
         <v>69</v>
@@ -3800,7 +3800,7 @@
         <v>30</v>
       </c>
       <c r="AC25" t="n">
-        <v>10.55431582842505</v>
+        <v>10.6</v>
       </c>
       <c r="AD25" t="n">
         <v>49</v>
@@ -4066,7 +4066,7 @@
         <v>27</v>
       </c>
       <c r="AC27" t="n">
-        <v>23.27080619094652</v>
+        <v>23.3</v>
       </c>
       <c r="AD27" t="n">
         <v>44</v>
@@ -4198,7 +4198,7 @@
         <v>34</v>
       </c>
       <c r="AC28" t="n">
-        <v>2.135392804604378</v>
+        <v>2.1</v>
       </c>
       <c r="AD28" t="n">
         <v>34</v>
@@ -4464,7 +4464,7 @@
         <v>29</v>
       </c>
       <c r="AC30" t="n">
-        <v>19.87750610974286</v>
+        <v>19.9</v>
       </c>
       <c r="AD30" t="n">
         <v>45</v>
@@ -5668,7 +5668,7 @@
         <v>24</v>
       </c>
       <c r="AC39" t="n">
-        <v>11.65937493450427</v>
+        <v>11.7</v>
       </c>
       <c r="AD39" t="n">
         <v>43</v>
@@ -5800,7 +5800,7 @@
         <v>34</v>
       </c>
       <c r="AC40" t="n">
-        <v>2.750202714525626</v>
+        <v>2.8</v>
       </c>
       <c r="AD40" t="n">
         <v>33</v>
@@ -6200,7 +6200,7 @@
         <v>24</v>
       </c>
       <c r="AC43" t="n">
-        <v>20.6046310640093</v>
+        <v>20.6</v>
       </c>
       <c r="AD43" t="n">
         <v>50</v>
@@ -6868,7 +6868,7 @@
         <v>24</v>
       </c>
       <c r="AC48" t="n">
-        <v>7.088065468401728</v>
+        <v>7.1</v>
       </c>
       <c r="AD48" t="n">
         <v>29</v>
@@ -7134,7 +7134,7 @@
         <v>21</v>
       </c>
       <c r="AC50" t="n">
-        <v>7.432311707948527</v>
+        <v>7.4</v>
       </c>
       <c r="AD50" t="n">
         <v>48</v>
@@ -7266,7 +7266,7 @@
         <v>24</v>
       </c>
       <c r="AC51" t="n">
-        <v>17.85123684454724</v>
+        <v>17.9</v>
       </c>
       <c r="AD51" t="n">
         <v>25</v>

</xml_diff>